<commit_message>
strategy_radial Psychopaths added, courtesy of the Rayman
</commit_message>
<xml_diff>
--- a/[gameplay]/strategy_radial/GTASA MTA PTPM Peds.xlsx
+++ b/[gameplay]/strategy_radial/GTASA MTA PTPM Peds.xlsx
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="224">
   <si>
     <t>SkinID</t>
   </si>
@@ -130,18 +130,12 @@
     <t>Prime Rib</t>
   </si>
   <si>
-    <t>BBC</t>
-  </si>
-  <si>
     <t>Beefy White Guy</t>
   </si>
   <si>
     <t>Token White Guy</t>
   </si>
   <si>
-    <t>Will Smiff</t>
-  </si>
-  <si>
     <t>Cop</t>
   </si>
   <si>
@@ -214,9 +208,6 @@
     <t>WMYBU</t>
   </si>
   <si>
-    <t>BMYMIB</t>
-  </si>
-  <si>
     <t>WMYAMMO</t>
   </si>
   <si>
@@ -617,13 +608,136 @@
   </si>
   <si>
     <t>18, 20, 51</t>
+  </si>
+  <si>
+    <t>OK WAIT, this is actually Will Smith but his files are missing (WMYMIB?) so its the other black bouncer guy</t>
+  </si>
+  <si>
+    <t>0, 4</t>
+  </si>
+  <si>
+    <t>36, 49, 50, 51</t>
+  </si>
+  <si>
+    <t>96, 97</t>
+  </si>
+  <si>
+    <t>3, 41</t>
+  </si>
+  <si>
+    <t>8, 10, 12, 18</t>
+  </si>
+  <si>
+    <t>65, 120, 121</t>
+  </si>
+  <si>
+    <t>1, 136, 137</t>
+  </si>
+  <si>
+    <t>27, 58</t>
+  </si>
+  <si>
+    <t>173, 174</t>
+  </si>
+  <si>
+    <t>125, 126, 127</t>
+  </si>
+  <si>
+    <t>128, 129, 130, 132</t>
+  </si>
+  <si>
+    <t>21, 90, 91</t>
+  </si>
+  <si>
+    <t>23, 61</t>
+  </si>
+  <si>
+    <t>9, 10, 100</t>
+  </si>
+  <si>
+    <t>28, 34</t>
+  </si>
+  <si>
+    <t>50, 51, 60</t>
+  </si>
+  <si>
+    <t>12, 26, 27, 28, 29, 30, 32, 43, 44, 46, 47, 59, 61, 69, 79, 83</t>
+  </si>
+  <si>
+    <t>15, 18, 31, 127, 128</t>
+  </si>
+  <si>
+    <t>88,  94</t>
+  </si>
+  <si>
+    <t>4, 89, 91, 92, 93</t>
+  </si>
+  <si>
+    <t>62, 77</t>
+  </si>
+  <si>
+    <t>21, 64, 67, 118</t>
+  </si>
+  <si>
+    <t>20, 114</t>
+  </si>
+  <si>
+    <t>23, 57, 58</t>
+  </si>
+  <si>
+    <t>22, 24, 32, 80, 83</t>
+  </si>
+  <si>
+    <t>14, 38, 62, 89</t>
+  </si>
+  <si>
+    <t>16, 109, 166</t>
+  </si>
+  <si>
+    <t>82, 122</t>
+  </si>
+  <si>
+    <t>33,  42, 115, 116</t>
+  </si>
+  <si>
+    <t>19, 20, 149, 167</t>
+  </si>
+  <si>
+    <t>0, 84, 93, 128</t>
+  </si>
+  <si>
+    <t>51, 111, 135</t>
+  </si>
+  <si>
+    <t>1, 47, 60, 118, 158, 160, 164</t>
+  </si>
+  <si>
+    <t>26, 90</t>
+  </si>
+  <si>
+    <t>61, 146, 156</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5, 78, 88 </t>
+  </si>
+  <si>
+    <t>playSFX("spc_ga", 132, 4, false)</t>
+  </si>
+  <si>
+    <t>playSFX("spc_ga", 44, 8, false)</t>
+  </si>
+  <si>
+    <t>playSFX("spc_ga", 153, 1, false)</t>
+  </si>
+  <si>
+    <t>playSFX("spc_ga", 134, 1, false)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -646,6 +760,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -657,13 +778,26 @@
       <name val="Courier New"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFE5CA"/>
+        <bgColor rgb="FFFBE5D6"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -675,20 +809,36 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard 2" xfId="1" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor rgb="FFFFE8E1"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -734,22 +884,14 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{870F105C-9944-434C-B278-15EB314A2F26}" name="Tabel1" displayName="Tabel1" ref="A1:R30" totalsRowShown="0">
   <autoFilter ref="A1:R30" xr:uid="{58535BD7-03E8-44BE-8B5F-7D62E943820E}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="Bodyguard"/>
-        <filter val="Cop"/>
-        <filter val="Prime Minister"/>
-        <filter val="Terrorist"/>
-      </filters>
-    </filterColumn>
     <filterColumn colId="4">
       <filters>
         <filter val="Yes"/>
       </filters>
     </filterColumn>
   </autoFilter>
-  <sortState ref="A2:Q28">
-    <sortCondition ref="A1:A30"/>
+  <sortState ref="A2:R28">
+    <sortCondition ref="B1:B30"/>
   </sortState>
   <tableColumns count="18">
     <tableColumn id="1" xr3:uid="{75EAF82F-75D0-4803-967B-E13A5D3BDBF9}" name="SkinID"/>
@@ -1075,7 +1217,7 @@
   <dimension ref="A1:R37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1098,220 +1240,190 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="K1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="N1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="R1" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="24" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>73</v>
+        <v>141</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>74</v>
+        <v>91</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="I2" s="2">
-        <v>15</v>
-      </c>
-      <c r="J2" s="2">
-        <v>9</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="L2" s="2">
-        <v>45</v>
-      </c>
-      <c r="M2" s="2">
-        <v>137</v>
+        <v>92</v>
+      </c>
+      <c r="H2" s="2">
+        <v>147</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="K2" s="2">
+        <v>171</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>88</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="O2" s="2">
-        <v>50</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>72</v>
+        <v>95</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="P2" s="2">
+        <v>51</v>
       </c>
       <c r="Q2" s="2">
-        <v>29</v>
+        <v>63</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" ht="24" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>100</v>
+        <v>163</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>47</v>
+        <v>18</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="N3" s="2">
+        <v>38</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="1" t="s">
         <v>114</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="Q3" s="2">
-        <v>80</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
+        <v>164</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="2">
+        <v>66.67</v>
+      </c>
+      <c r="G4" s="2">
+        <v>4</v>
+      </c>
+      <c r="H4" s="2">
+        <v>85</v>
+      </c>
+      <c r="I4" s="2">
+        <v>53</v>
+      </c>
+      <c r="J4" s="2">
+        <v>57</v>
+      </c>
+      <c r="K4" s="2">
+        <v>81</v>
+      </c>
+      <c r="L4" s="2">
+        <v>87</v>
+      </c>
+      <c r="M4" s="2">
+        <v>79</v>
+      </c>
+      <c r="N4" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F4" s="2">
-        <v>0</v>
-      </c>
-      <c r="G4" s="2">
+      <c r="O4" s="2">
+        <v>32</v>
+      </c>
+      <c r="P4" s="2">
         <v>19</v>
       </c>
-      <c r="H4" s="2">
-        <v>7</v>
-      </c>
-      <c r="I4" s="2">
-        <v>7</v>
-      </c>
-      <c r="J4" s="2">
-        <v>3</v>
-      </c>
-      <c r="K4" s="2">
+      <c r="Q4" s="2">
         <v>17</v>
       </c>
-      <c r="L4" s="2">
-        <v>18</v>
-      </c>
-      <c r="M4" s="2">
-        <v>1</v>
-      </c>
-      <c r="N4" s="2">
-        <v>2</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="P4" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="Q4" s="2">
-        <v>6</v>
-      </c>
       <c r="R4" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="96" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>137</v>
       </c>
@@ -1322,585 +1434,612 @@
         <v>14</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2"/>
-      <c r="P5" s="2"/>
-      <c r="Q5" s="2"/>
-    </row>
-    <row r="6" spans="1:18" ht="24" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="K5" s="3">
+        <v>73</v>
+      </c>
+      <c r="L5" s="3">
+        <v>119</v>
+      </c>
+      <c r="M5" s="3">
+        <v>16</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="Q5" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="R5" s="4" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>141</v>
+        <v>165</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="2">
+        <v>5</v>
+      </c>
+      <c r="G6" s="2">
+        <v>22</v>
+      </c>
+      <c r="H6" s="2">
+        <v>31</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="J6" s="2">
+        <v>30</v>
+      </c>
+      <c r="K6" s="2">
+        <v>31</v>
+      </c>
+      <c r="L6" s="2">
+        <v>35</v>
+      </c>
+      <c r="M6" s="2">
+        <v>36</v>
+      </c>
+      <c r="N6" s="2">
+        <v>29</v>
+      </c>
+      <c r="O6" s="2">
+        <v>38</v>
+      </c>
+      <c r="P6" s="2">
+        <v>10</v>
+      </c>
+      <c r="Q6" s="2">
+        <v>20</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>166</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F6" s="2" t="s">
+      <c r="E7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="H7" s="2">
+        <v>60</v>
+      </c>
+      <c r="I7" s="2">
+        <v>61</v>
+      </c>
+      <c r="J7" s="2">
+        <v>63</v>
+      </c>
+      <c r="K7" s="2">
+        <v>90</v>
+      </c>
+      <c r="L7" s="2">
+        <v>72</v>
+      </c>
+      <c r="M7" s="2">
+        <v>47</v>
+      </c>
+      <c r="N7" s="2">
         <v>94</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="H6" s="2">
-        <v>147</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="K6" s="2">
-        <v>171</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="M6" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="N6" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="O6" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="P6" s="2">
-        <v>51</v>
-      </c>
-      <c r="Q6" s="2">
-        <v>63</v>
-      </c>
-      <c r="R6" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" ht="24" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>147</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="L7" s="2" t="s">
+      <c r="O7" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="M7" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="N7" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="O7" s="2">
-        <v>99</v>
-      </c>
       <c r="P7" s="2">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="Q7" s="2">
-        <v>104</v>
+        <v>73</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>100</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>163</v>
+        <v>276</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>43</v>
+        <v>156</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>116</v>
+        <v>37</v>
+      </c>
+      <c r="F8" s="2">
+        <v>58</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>114</v>
+        <v>167</v>
       </c>
       <c r="H8" s="2">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="I8" s="2">
-        <v>61</v>
+        <v>41</v>
       </c>
       <c r="J8" s="2">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="K8" s="2">
-        <v>90</v>
+        <v>47</v>
       </c>
       <c r="L8" s="2">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="M8" s="2">
-        <v>47</v>
-      </c>
-      <c r="N8" s="2">
-        <v>94</v>
+        <v>38</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>168</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="P8" s="2">
-        <v>27</v>
+        <v>166</v>
+      </c>
+      <c r="P8" s="2" t="s">
+        <v>165</v>
       </c>
       <c r="Q8" s="2">
-        <v>73</v>
+        <v>1</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>117</v>
+        <v>169</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>164</v>
+        <v>246</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F9" s="2">
-        <v>66.67</v>
+        <v>10</v>
       </c>
       <c r="G9" s="2">
+        <v>5</v>
+      </c>
+      <c r="H9" s="2">
+        <v>1</v>
+      </c>
+      <c r="I9" s="2">
+        <v>13</v>
+      </c>
+      <c r="J9" s="2">
         <v>4</v>
       </c>
-      <c r="H9" s="2">
-        <v>85</v>
-      </c>
-      <c r="I9" s="2">
-        <v>53</v>
-      </c>
-      <c r="J9" s="2">
-        <v>57</v>
-      </c>
       <c r="K9" s="2">
-        <v>81</v>
+        <v>3</v>
       </c>
       <c r="L9" s="2">
-        <v>87</v>
+        <v>2</v>
       </c>
       <c r="M9" s="2">
-        <v>79</v>
-      </c>
-      <c r="N9" s="2" t="s">
-        <v>114</v>
+        <v>0</v>
+      </c>
+      <c r="N9" s="2">
+        <v>6</v>
       </c>
       <c r="O9" s="2">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="P9" s="2">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="Q9" s="2">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>120</v>
+        <v>154</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>165</v>
+        <v>275</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" s="2">
+        <v>24</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="H10" s="2">
+        <v>57</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="J10" s="2">
+        <v>1</v>
+      </c>
+      <c r="K10" s="2">
+        <v>48</v>
+      </c>
+      <c r="L10" s="2">
+        <v>61</v>
+      </c>
+      <c r="M10" s="2">
+        <v>44</v>
+      </c>
+      <c r="N10" s="2">
         <v>18</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F10" s="2">
-        <v>5</v>
-      </c>
-      <c r="G10" s="2">
-        <v>22</v>
-      </c>
-      <c r="H10" s="2">
-        <v>31</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="J10" s="2">
-        <v>30</v>
-      </c>
-      <c r="K10" s="2">
-        <v>31</v>
-      </c>
-      <c r="L10" s="2">
-        <v>35</v>
-      </c>
-      <c r="M10" s="2">
-        <v>36</v>
-      </c>
-      <c r="N10" s="2">
-        <v>29</v>
-      </c>
       <c r="O10" s="2">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="P10" s="2">
-        <v>10</v>
-      </c>
-      <c r="Q10" s="2">
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c r="Q10" s="2" t="s">
+        <v>163</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>118</v>
+        <v>170</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>166</v>
+        <v>281</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>51</v>
+        <v>171</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F11" s="2">
-        <v>5</v>
+        <v>37</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>136</v>
       </c>
       <c r="G11" s="2">
-        <v>22</v>
-      </c>
-      <c r="H11" s="2">
-        <v>31</v>
+        <v>0</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>175</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="J11" s="2">
-        <v>30</v>
+        <v>178</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>177</v>
       </c>
       <c r="K11" s="2">
-        <v>31</v>
+        <v>92</v>
       </c>
       <c r="L11" s="2">
-        <v>35</v>
+        <v>66</v>
       </c>
       <c r="M11" s="2">
-        <v>36</v>
-      </c>
-      <c r="N11" s="2">
-        <v>29</v>
-      </c>
-      <c r="O11" s="2">
-        <v>38</v>
-      </c>
-      <c r="P11" s="2">
-        <v>10</v>
+        <v>77</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="O11" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="P11" s="2" t="s">
+        <v>174</v>
       </c>
       <c r="Q11" s="2">
-        <v>20</v>
+        <v>97</v>
       </c>
       <c r="R11" s="1" t="s">
-        <v>118</v>
+        <v>172</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
+        <v>285</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F12" s="2">
+        <v>27</v>
+      </c>
+      <c r="G12" s="2">
+        <v>42</v>
+      </c>
+      <c r="H12" s="2">
+        <v>37</v>
+      </c>
+      <c r="I12" s="2">
+        <v>19</v>
+      </c>
+      <c r="J12" s="2">
+        <v>18</v>
+      </c>
+      <c r="K12" s="2">
+        <v>8</v>
+      </c>
+      <c r="L12" s="2">
+        <v>13</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="N12" s="2">
+        <v>20</v>
+      </c>
+      <c r="O12" s="2">
+        <v>2</v>
+      </c>
+      <c r="P12" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="2">
+        <v>1</v>
+      </c>
+      <c r="R12" s="1" t="s">
         <v>179</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="H12" s="2">
-        <v>36</v>
-      </c>
-      <c r="I12" s="2">
-        <v>11</v>
-      </c>
-      <c r="J12" s="2">
-        <v>3</v>
-      </c>
-      <c r="K12" s="2">
-        <v>74</v>
-      </c>
-      <c r="L12" s="2">
-        <v>9</v>
-      </c>
-      <c r="M12" s="2">
-        <v>28</v>
-      </c>
-      <c r="N12" s="2">
-        <v>37</v>
-      </c>
-      <c r="O12" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="P12" s="2">
-        <v>40</v>
-      </c>
-      <c r="Q12" s="2">
-        <v>49</v>
-      </c>
-      <c r="R12" s="1" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="24" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>181</v>
+        <v>147</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>136</v>
+        <v>107</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>130</v>
+        <v>102</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>133</v>
+        <v>103</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>134</v>
+        <v>105</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="K13" s="2">
-        <v>4</v>
-      </c>
-      <c r="L13" s="2">
-        <v>45</v>
+        <v>106</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>109</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="N13" s="2">
-        <v>83</v>
-      </c>
-      <c r="O13" s="2" t="s">
-        <v>132</v>
+        <v>110</v>
+      </c>
+      <c r="N13" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="O13" s="2">
+        <v>99</v>
       </c>
       <c r="P13" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q13" s="2" t="s">
-        <v>131</v>
+        <v>15</v>
+      </c>
+      <c r="Q13" s="2">
+        <v>104</v>
       </c>
       <c r="R13" s="1" t="s">
-        <v>125</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:18" ht="24" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>183</v>
+        <v>73</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="G14" s="2">
-        <v>104</v>
+        <v>71</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>182</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>144</v>
+        <v>73</v>
       </c>
       <c r="I14" s="2">
-        <v>155</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>145</v>
+        <v>15</v>
+      </c>
+      <c r="J14" s="2">
+        <v>9</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>148</v>
+        <v>74</v>
       </c>
       <c r="L14" s="2">
-        <v>222</v>
-      </c>
-      <c r="M14" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="N14" s="2">
-        <v>199</v>
-      </c>
-      <c r="O14" s="2" t="s">
-        <v>143</v>
+        <v>45</v>
+      </c>
+      <c r="M14" s="2">
+        <v>137</v>
+      </c>
+      <c r="N14" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="O14" s="2">
+        <v>50</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>142</v>
+        <v>69</v>
       </c>
       <c r="Q14" s="2">
-        <v>103</v>
+        <v>29</v>
       </c>
       <c r="R14" s="1" t="s">
-        <v>138</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:18" ht="24" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>191</v>
+        <v>100</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>150</v>
+        <v>45</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>155</v>
+        <v>85</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="H15" s="2">
-        <v>117</v>
+        <v>77</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>82</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>153</v>
+        <v>83</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="K15" s="2">
-        <v>363</v>
-      </c>
-      <c r="L15" s="2">
-        <v>360</v>
-      </c>
-      <c r="M15" s="2">
-        <v>210</v>
-      </c>
-      <c r="N15" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="O15" s="2">
-        <v>262</v>
-      </c>
-      <c r="P15" s="2">
-        <v>345</v>
-      </c>
-      <c r="Q15" s="2" t="s">
-        <v>156</v>
+        <v>84</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="N15" s="2">
+        <v>114</v>
+      </c>
+      <c r="O15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="P15" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q15" s="2">
+        <v>80</v>
       </c>
       <c r="R15" s="1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" ht="24" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>200</v>
       </c>
@@ -1911,25 +2050,52 @@
         <v>15</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
-      <c r="O16" s="2"/>
-      <c r="P16" s="2"/>
-      <c r="Q16" s="2"/>
-    </row>
-    <row r="17" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="L16" s="3">
+        <v>60</v>
+      </c>
+      <c r="M16" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="N16" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="O16" s="3">
+        <v>7</v>
+      </c>
+      <c r="P16" s="3">
+        <v>24</v>
+      </c>
+      <c r="Q16" s="3">
+        <v>26</v>
+      </c>
+      <c r="R16" s="5" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" ht="24" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>212</v>
       </c>
@@ -1940,27 +2106,54 @@
         <v>16</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="2"/>
-      <c r="M17" s="2"/>
-      <c r="N17" s="2"/>
-      <c r="O17" s="2"/>
-      <c r="P17" s="2"/>
-      <c r="Q17" s="2"/>
-    </row>
-    <row r="18" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="K17" s="3">
+        <v>19</v>
+      </c>
+      <c r="L17" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="M17" s="3">
+        <v>43</v>
+      </c>
+      <c r="N17" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="O17" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="P17" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="Q17" s="3">
+        <v>86</v>
+      </c>
+      <c r="R17" s="5" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" ht="36" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>230</v>
+        <v>130</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>13</v>
@@ -1969,246 +2162,273 @@
         <v>17</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
-      <c r="O18" s="2"/>
-      <c r="P18" s="2"/>
-      <c r="Q18" s="2"/>
+        <v>37</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="L18" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="M18" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="N18" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="O18" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="P18" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="Q18" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="R18" s="6" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>246</v>
+        <v>111</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>27</v>
+        <v>4</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F19" s="2">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G19" s="2">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="H19" s="2">
+        <v>7</v>
+      </c>
+      <c r="I19" s="2">
+        <v>7</v>
+      </c>
+      <c r="J19" s="2">
+        <v>3</v>
+      </c>
+      <c r="K19" s="2">
+        <v>17</v>
+      </c>
+      <c r="L19" s="2">
+        <v>18</v>
+      </c>
+      <c r="M19" s="2">
         <v>1</v>
       </c>
-      <c r="I19" s="2">
-        <v>13</v>
-      </c>
-      <c r="J19" s="2">
-        <v>4</v>
-      </c>
-      <c r="K19" s="2">
-        <v>3</v>
-      </c>
-      <c r="L19" s="2">
+      <c r="N19" s="2">
         <v>2</v>
       </c>
-      <c r="M19" s="2">
-        <v>0</v>
-      </c>
-      <c r="N19" s="2">
+      <c r="O19" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="P19" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q19" s="2">
         <v>6</v>
       </c>
-      <c r="O19" s="2">
-        <v>8</v>
-      </c>
-      <c r="P19" s="2">
-        <v>7</v>
-      </c>
-      <c r="Q19" s="2">
-        <v>11</v>
-      </c>
       <c r="R19" s="1" t="s">
-        <v>157</v>
+        <v>99</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>274</v>
+        <v>179</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>160</v>
+        <v>49</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="G20" s="2">
+        <v>121</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="H20" s="2">
+        <v>36</v>
+      </c>
+      <c r="I20" s="2">
+        <v>11</v>
+      </c>
+      <c r="J20" s="2">
+        <v>3</v>
+      </c>
+      <c r="K20" s="2">
+        <v>74</v>
+      </c>
+      <c r="L20" s="2">
+        <v>9</v>
+      </c>
+      <c r="M20" s="2">
+        <v>28</v>
+      </c>
+      <c r="N20" s="2">
+        <v>37</v>
+      </c>
+      <c r="O20" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="P20" s="2">
+        <v>40</v>
+      </c>
+      <c r="Q20" s="2">
+        <v>49</v>
+      </c>
+      <c r="R20" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" ht="24" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>181</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="K21" s="2">
+        <v>4</v>
+      </c>
+      <c r="L21" s="2">
+        <v>45</v>
+      </c>
+      <c r="M21" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="N21" s="2">
+        <v>83</v>
+      </c>
+      <c r="O21" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="P21" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q21" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="R21" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" ht="24" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>183</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H20" s="2">
-        <v>22</v>
-      </c>
-      <c r="I20" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="J20" s="2">
-        <v>9</v>
-      </c>
-      <c r="K20" s="2">
-        <v>36</v>
-      </c>
-      <c r="L20" s="2">
-        <v>35</v>
-      </c>
-      <c r="M20" s="2">
-        <v>4</v>
-      </c>
-      <c r="N20" s="2">
-        <v>25</v>
-      </c>
-      <c r="O20" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="P20" s="2">
-        <v>13</v>
-      </c>
-      <c r="Q20" s="2">
-        <v>24</v>
-      </c>
-      <c r="R20" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
-        <v>275</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F21" s="2">
-        <v>24</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="H21" s="2">
-        <v>57</v>
-      </c>
-      <c r="I21" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="J21" s="2">
-        <v>1</v>
-      </c>
-      <c r="K21" s="2">
-        <v>48</v>
-      </c>
-      <c r="L21" s="2">
-        <v>61</v>
-      </c>
-      <c r="M21" s="2">
-        <v>44</v>
-      </c>
-      <c r="N21" s="2">
-        <v>18</v>
-      </c>
-      <c r="O21" s="2">
-        <v>17</v>
-      </c>
-      <c r="P21" s="2">
-        <v>21</v>
-      </c>
-      <c r="Q21" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="R21" s="1" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <v>276</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="D22" s="1" t="s">
-        <v>159</v>
+        <v>51</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F22" s="2">
-        <v>58</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="H22" s="2">
-        <v>61</v>
+        <v>37</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="G22" s="2">
+        <v>104</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>141</v>
       </c>
       <c r="I22" s="2">
-        <v>41</v>
-      </c>
-      <c r="J22" s="2">
-        <v>42</v>
-      </c>
-      <c r="K22" s="2">
-        <v>47</v>
+        <v>155</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>145</v>
       </c>
       <c r="L22" s="2">
-        <v>48</v>
-      </c>
-      <c r="M22" s="2">
-        <v>38</v>
-      </c>
-      <c r="N22" s="2" t="s">
-        <v>171</v>
+        <v>222</v>
+      </c>
+      <c r="M22" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="N22" s="2">
+        <v>199</v>
       </c>
       <c r="O22" s="2" t="s">
-        <v>169</v>
+        <v>140</v>
       </c>
       <c r="P22" s="2" t="s">
-        <v>168</v>
+        <v>139</v>
       </c>
       <c r="Q22" s="2">
-        <v>1</v>
+        <v>103</v>
       </c>
       <c r="R22" s="1" t="s">
-        <v>172</v>
+        <v>135</v>
       </c>
     </row>
     <row r="23" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
@@ -2216,72 +2436,72 @@
         <v>280</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" ht="24" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>281</v>
+        <v>191</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>27</v>
+        <v>4</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>174</v>
+        <v>147</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="G24" s="2">
-        <v>0</v>
-      </c>
-      <c r="H24" s="2" t="s">
-        <v>178</v>
+        <v>152</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="H24" s="2">
+        <v>117</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>181</v>
+        <v>150</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>180</v>
+        <v>151</v>
       </c>
       <c r="K24" s="2">
-        <v>92</v>
+        <v>363</v>
       </c>
       <c r="L24" s="2">
-        <v>66</v>
+        <v>360</v>
       </c>
       <c r="M24" s="2">
-        <v>77</v>
+        <v>210</v>
       </c>
       <c r="N24" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="O24" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="P24" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="Q24" s="2">
-        <v>97</v>
+        <v>149</v>
+      </c>
+      <c r="O24" s="2">
+        <v>262</v>
+      </c>
+      <c r="P24" s="2">
+        <v>345</v>
+      </c>
+      <c r="Q24" s="2" t="s">
+        <v>153</v>
       </c>
       <c r="R24" s="1" t="s">
-        <v>175</v>
+        <v>146</v>
       </c>
     </row>
     <row r="25" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
@@ -2289,16 +2509,16 @@
         <v>282</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
@@ -2306,16 +2526,16 @@
         <v>283</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
@@ -2323,72 +2543,72 @@
         <v>284</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>285</v>
+        <v>274</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>27</v>
+        <v>4</v>
       </c>
       <c r="C28" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="G28" s="2">
+        <v>10</v>
+      </c>
+      <c r="H28" s="2">
+        <v>22</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="J28" s="2">
+        <v>9</v>
+      </c>
+      <c r="K28" s="2">
+        <v>36</v>
+      </c>
+      <c r="L28" s="2">
         <v>35</v>
       </c>
-      <c r="D28" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F28" s="2">
-        <v>27</v>
-      </c>
-      <c r="G28" s="2">
-        <v>42</v>
-      </c>
-      <c r="H28" s="2">
-        <v>37</v>
-      </c>
-      <c r="I28" s="2">
-        <v>19</v>
-      </c>
-      <c r="J28" s="2">
-        <v>18</v>
-      </c>
-      <c r="K28" s="2">
-        <v>8</v>
-      </c>
-      <c r="L28" s="2">
+      <c r="M28" s="2">
+        <v>4</v>
+      </c>
+      <c r="N28" s="2">
+        <v>25</v>
+      </c>
+      <c r="O28" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="P28" s="2">
         <v>13</v>
       </c>
-      <c r="M28" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="N28" s="2">
-        <v>20</v>
-      </c>
-      <c r="O28" s="2">
-        <v>2</v>
-      </c>
-      <c r="P28" s="2">
-        <v>0</v>
-      </c>
       <c r="Q28" s="2">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="R28" s="1" t="s">
-        <v>182</v>
+        <v>158</v>
       </c>
     </row>
     <row r="29" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
@@ -2396,16 +2616,16 @@
         <v>286</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="30" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
@@ -2413,56 +2633,61 @@
         <v>288</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="35" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C35" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="36" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C36" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="37" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C37" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="F2:Q9 F12:Q28">
-    <cfRule type="notContainsBlanks" dxfId="2" priority="3">
+  <conditionalFormatting sqref="F2:Q6 F12:Q28 F8:Q9">
+    <cfRule type="notContainsBlanks" dxfId="3" priority="7">
       <formula>LEN(TRIM(F2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F10:Q10">
-    <cfRule type="notContainsBlanks" dxfId="1" priority="2">
+    <cfRule type="notContainsBlanks" dxfId="2" priority="6">
       <formula>LEN(TRIM(F10))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F11:Q11">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="1">
+    <cfRule type="notContainsBlanks" dxfId="1" priority="5">
       <formula>LEN(TRIM(F11))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F7:Q7">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="4">
+      <formula>LEN(TRIM(F7))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>